<commit_message>
WIP - get doc type
work in progress for getting the type of document based on country and
kind code CAKC and doc length type DLT
</commit_message>
<xml_diff>
--- a/inst/extdata/docLengthTypes.xlsx
+++ b/inst/extdata/docLengthTypes.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="18">
   <si>
     <t>key</t>
   </si>
@@ -72,6 +72,12 @@
   </si>
   <si>
     <t>JPWO10</t>
+  </si>
+  <si>
+    <t>JPH7</t>
+  </si>
+  <si>
+    <t>JP7</t>
   </si>
 </sst>
 </file>
@@ -386,10 +392,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -482,6 +488,22 @@
         <v>11</v>
       </c>
     </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13" t="s">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>